<commit_message>
`Updated expense_details.xlsx and income_details.xlsx files`
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,95 +416,29 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>electricity</v>
+        <v>rent</v>
       </c>
       <c r="B2">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="C2" s="1">
-        <v>45778.125185185185</v>
+        <v>45782.125185185185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>rent</v>
+        <v>fuel</v>
       </c>
       <c r="B3">
-        <v>3000</v>
+        <v>20000</v>
       </c>
       <c r="C3" s="1">
-        <v>45777.125185185185</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Groceries</v>
-      </c>
-      <c r="B4">
-        <v>3000</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45777.125185185185</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Personal utilities</v>
-      </c>
-      <c r="B5">
-        <v>5000</v>
-      </c>
-      <c r="C5" s="1">
-        <v>45777.125185185185</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Gas</v>
-      </c>
-      <c r="B6">
-        <v>2000</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45777.125185185185</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Water bill</v>
-      </c>
-      <c r="B7">
-        <v>2000</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45777.125185185185</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Fuel</v>
-      </c>
-      <c r="B8">
-        <v>1500</v>
-      </c>
-      <c r="C8" s="1">
-        <v>45777.125185185185</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Electricity bill</v>
-      </c>
-      <c r="B9">
-        <v>1500</v>
-      </c>
-      <c r="C9" s="1">
-        <v>45777.125185185185</v>
+        <v>45782.125185185185</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>